<commit_message>
[FEATURE] working on import
</commit_message>
<xml_diff>
--- a/Hydra/Hydra.Import.Test/Resources/Import001.xlsx
+++ b/Hydra/Hydra.Import.Test/Resources/Import001.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Meta" sheetId="1" r:id="rId1"/>
+    <sheet name="Meta" sheetId="2" r:id="rId1"/>
+    <sheet name="Resources" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,15 +25,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Mappings</t>
-  </si>
-  <si>
-    <t>Foo</t>
-  </si>
-  <si>
-    <t>Hydra.Import.Test.Foo</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Assembly Qualified Type Name</t>
+  </si>
+  <si>
+    <t>Hydra.Nh.Infrastructure.I18n.ResourceItem, Hydra.Nh</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>TwoLetterISOLanguageName</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>FOO_DE</t>
+  </si>
+  <si>
+    <t>FOO</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>FOO_EN</t>
+  </si>
+  <si>
+    <t>BAR.BAZ</t>
+  </si>
+  <si>
+    <t>BAR.BAZ_DE</t>
+  </si>
+  <si>
+    <t>BAR.BAZ_EN</t>
   </si>
 </sst>
 </file>
@@ -361,28 +398,106 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[UPDATE] can import types and read meta sheet
</commit_message>
<xml_diff>
--- a/Hydra/Hydra.Import.Test/Resources/Import001.xlsx
+++ b/Hydra/Hydra.Import.Test/Resources/Import001.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="2" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>Sheet</t>
   </si>
   <si>
-    <t>Assembly Qualified Type Name</t>
-  </si>
-  <si>
     <t>Hydra.Nh.Infrastructure.I18n.ResourceItem, Hydra.Nh</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>BAR.BAZ_EN</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -398,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -420,7 +420,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -433,7 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -444,57 +444,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[CLEAN] fixed tests and moved in memory db config to reusable extension
</commit_message>
<xml_diff>
--- a/Hydra/Hydra.Import.Test/Resources/Import001.xlsx
+++ b/Hydra/Hydra.Import.Test/Resources/Import001.xlsx
@@ -33,9 +33,6 @@
     <t>Sheet</t>
   </si>
   <si>
-    <t>Hydra.Nh.Infrastructure.I18n.ResourceItem, Hydra.Nh</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Hydra.Infrastructure.I18n.ResourceItem, Hydra.Infrastructure</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -420,7 +420,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -444,57 +444,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] lets write resource items to resx files :)
</commit_message>
<xml_diff>
--- a/Hydra/Hydra.Import.Test/Resources/Import001.xlsx
+++ b/Hydra/Hydra.Import.Test/Resources/Import001.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="2" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>TwoLetterISOLanguageName</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Hydra.Infrastructure.I18n.ResourceItem, Hydra.Infrastructure</t>
+  </si>
+  <si>
+    <t>Language</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -412,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -420,7 +420,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,54 +447,54 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>